<commit_message>
Added Trained Dataset (1/4)
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Desktop\Pytomation\Assignment\Mathematics in the Modern World\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Desktop\Pytomation\Frequency Distribution Table\Frequency-Distribution-Table-Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -522,7 +522,7 @@
   <dimension ref="A1:AE101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +655,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>12.78</v>
+        <v>9.7100000000000009</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -690,7 +690,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>13.17</v>
+        <v>9.83</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>13.44</v>
+        <v>10.08</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -760,7 +760,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>13.44</v>
+        <v>11.32</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -830,7 +830,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>13.48</v>
+        <v>13.52</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -865,7 +865,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>14.19</v>
+        <v>14.12</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -900,7 +900,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>15.1</v>
+        <v>15.89</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -935,7 +935,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>15.18</v>
+        <v>16.09</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -970,7 +970,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>16.170000000000002</v>
+        <v>17.34</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>16.18</v>
+        <v>18.48</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>17.190000000000001</v>
+        <v>18.52</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>18.21</v>
+        <v>18.670000000000002</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>19.22</v>
+        <v>19.05</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>20.22</v>
+        <v>19.13</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>21.14</v>
+        <v>20.14</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>21.17</v>
+        <v>21</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>21.19</v>
+        <v>21.17</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>22.17</v>
+        <v>21.83</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>22.18</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>22.24</v>
+        <v>22.61</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>23.16</v>
+        <v>22.89</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>23.18</v>
+        <v>23.08</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1460,7 +1460,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>24.18</v>
+        <v>23.38</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>24.18</v>
+        <v>23.42</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>25.14</v>
+        <v>23.7</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>25.16</v>
+        <v>23.8</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>26.16</v>
+        <v>24.31</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>26.18</v>
+        <v>24.62</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>27.19</v>
+        <v>24.73</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>27.19</v>
+        <v>24.88</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>28.08</v>
+        <v>25.08</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>28.11</v>
+        <v>25.12</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>29.31</v>
+        <v>25.21</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>29.31</v>
+        <v>25.64</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1880,7 +1880,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>30.1</v>
+        <v>26.01</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>30.12</v>
+        <v>26.17</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>31.18</v>
+        <v>26.21</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>31.21</v>
+        <v>26.41</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>31.34</v>
+        <v>26.87</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>31.45</v>
+        <v>27.13</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2090,7 +2090,7 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>31.52</v>
+        <v>27.33</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -2125,7 +2125,7 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>32.159999999999997</v>
+        <v>27.42</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -2160,7 +2160,7 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>32.17</v>
+        <v>27.53</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>32.18</v>
+        <v>27.91</v>
       </c>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -2230,7 +2230,7 @@
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>32.68</v>
+        <v>28.09</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -2265,7 +2265,7 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>33.119999999999997</v>
+        <v>28.18</v>
       </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -2300,7 +2300,7 @@
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>33.24</v>
+        <v>28.31</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -2335,7 +2335,7 @@
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>33.28</v>
+        <v>28.42</v>
       </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -2370,7 +2370,7 @@
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>34.159999999999997</v>
+        <v>28.48</v>
       </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
-        <v>34.18</v>
+        <v>29</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -2440,7 +2440,7 @@
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
-        <v>35.14</v>
+        <v>30.32</v>
       </c>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
-        <v>35.18</v>
+        <v>31.12</v>
       </c>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
-        <v>36.18</v>
+        <v>32.33</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
-        <v>36.200000000000003</v>
+        <v>32.33</v>
       </c>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
-        <v>37.119999999999997</v>
+        <v>33.450000000000003</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
-        <v>37.18</v>
+        <v>34.42</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
-        <v>37.24</v>
+        <v>35.89</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -2685,7 +2685,7 @@
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
-        <v>38.159999999999997</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -2720,7 +2720,7 @@
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
-        <v>38.33</v>
+        <v>38.450000000000003</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
-        <v>39.119999999999997</v>
+        <v>39.08</v>
       </c>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -2790,7 +2790,7 @@
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
-        <v>39.42</v>
+        <v>40.08</v>
       </c>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -2825,7 +2825,7 @@
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
-        <v>40.159999999999997</v>
+        <v>41.76</v>
       </c>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -2860,7 +2860,7 @@
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
-        <v>40.24</v>
+        <v>42.67</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -2894,9 +2894,7 @@
       <c r="AE65" s="5"/>
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A66" s="5">
-        <v>41.14</v>
-      </c>
+      <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -2929,9 +2927,7 @@
       <c r="AE66" s="5"/>
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
-        <v>41.33</v>
-      </c>
+      <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -2964,9 +2960,7 @@
       <c r="AE67" s="5"/>
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A68" s="5">
-        <v>42.08</v>
-      </c>
+      <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -2999,9 +2993,7 @@
       <c r="AE68" s="5"/>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
-        <v>42.12</v>
-      </c>
+      <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -3034,9 +3026,7 @@
       <c r="AE69" s="5"/>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A70" s="5">
-        <v>42.39</v>
-      </c>
+      <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -3069,9 +3059,7 @@
       <c r="AE70" s="5"/>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
-        <v>43.11</v>
-      </c>
+      <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -3104,9 +3092,7 @@
       <c r="AE71" s="5"/>
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A72" s="5">
-        <v>43.28</v>
-      </c>
+      <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -3139,9 +3125,7 @@
       <c r="AE72" s="5"/>
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A73" s="5">
-        <v>44.1</v>
-      </c>
+      <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -3174,9 +3158,7 @@
       <c r="AE73" s="5"/>
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A74" s="5">
-        <v>44.18</v>
-      </c>
+      <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -3209,9 +3191,7 @@
       <c r="AE74" s="5"/>
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A75" s="5">
-        <v>44.38</v>
-      </c>
+      <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -3244,9 +3224,7 @@
       <c r="AE75" s="5"/>
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A76" s="5">
-        <v>45.1</v>
-      </c>
+      <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -3279,9 +3257,7 @@
       <c r="AE76" s="5"/>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
-        <v>45.13</v>
-      </c>
+      <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -3314,9 +3290,7 @@
       <c r="AE77" s="5"/>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A78" s="5">
-        <v>45.83</v>
-      </c>
+      <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -3349,9 +3323,7 @@
       <c r="AE78" s="5"/>
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A79" s="5">
-        <v>46.13</v>
-      </c>
+      <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
@@ -3384,9 +3356,7 @@
       <c r="AE79" s="5"/>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A80" s="5">
-        <v>46.17</v>
-      </c>
+      <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
@@ -3419,9 +3389,7 @@
       <c r="AE80" s="5"/>
     </row>
     <row r="81" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A81" s="5">
-        <v>46.27</v>
-      </c>
+      <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
@@ -3454,9 +3422,7 @@
       <c r="AE81" s="5"/>
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A82" s="5">
-        <v>47.12</v>
-      </c>
+      <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
@@ -3489,9 +3455,7 @@
       <c r="AE82" s="5"/>
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A83" s="5">
-        <v>47.19</v>
-      </c>
+      <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
@@ -3524,9 +3488,7 @@
       <c r="AE83" s="5"/>
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A84" s="5">
-        <v>47.62</v>
-      </c>
+      <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -3559,9 +3521,7 @@
       <c r="AE84" s="5"/>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
-        <v>48.09</v>
-      </c>
+      <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
@@ -3594,9 +3554,7 @@
       <c r="AE85" s="5"/>
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A86" s="5">
-        <v>48.11</v>
-      </c>
+      <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -3629,9 +3587,7 @@
       <c r="AE86" s="5"/>
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A87" s="5">
-        <v>48.16</v>
-      </c>
+      <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
@@ -3664,9 +3620,7 @@
       <c r="AE87" s="5"/>
     </row>
     <row r="88" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A88" s="5">
-        <v>49.15</v>
-      </c>
+      <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -3699,9 +3653,7 @@
       <c r="AE88" s="5"/>
     </row>
     <row r="89" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
-        <v>49.9</v>
-      </c>
+      <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -3734,9 +3686,7 @@
       <c r="AE89" s="5"/>
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A90" s="5">
-        <v>50.11</v>
-      </c>
+      <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -3769,9 +3719,7 @@
       <c r="AE90" s="5"/>
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A91" s="5">
-        <v>50.11</v>
-      </c>
+      <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -3804,9 +3752,7 @@
       <c r="AE91" s="5"/>
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A92" s="5">
-        <v>51.14</v>
-      </c>
+      <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -3839,9 +3785,7 @@
       <c r="AE92" s="5"/>
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A93" s="5">
-        <v>51.18</v>
-      </c>
+      <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
@@ -3874,9 +3818,7 @@
       <c r="AE93" s="5"/>
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A94" s="5">
-        <v>52.18</v>
-      </c>
+      <c r="A94" s="5"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -3909,9 +3851,7 @@
       <c r="AE94" s="5"/>
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A95" s="5">
-        <v>52.18</v>
-      </c>
+      <c r="A95" s="5"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -3944,9 +3884,7 @@
       <c r="AE95" s="5"/>
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A96" s="5">
-        <v>53.1</v>
-      </c>
+      <c r="A96" s="5"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -3979,9 +3917,7 @@
       <c r="AE96" s="5"/>
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A97" s="5">
-        <v>53.17</v>
-      </c>
+      <c r="A97" s="5"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -4014,9 +3950,7 @@
       <c r="AE97" s="5"/>
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A98" s="5">
-        <v>54.18</v>
-      </c>
+      <c r="A98" s="5"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -4049,9 +3983,7 @@
       <c r="AE98" s="5"/>
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A99" s="5">
-        <v>54.18</v>
-      </c>
+      <c r="A99" s="5"/>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -4084,9 +4016,7 @@
       <c r="AE99" s="5"/>
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A100" s="5">
-        <v>55.53</v>
-      </c>
+      <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -4119,9 +4049,7 @@
       <c r="AE100" s="5"/>
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A101" s="5">
-        <v>62.17</v>
-      </c>
+      <c r="A101" s="5"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
@@ -4154,7 +4082,7 @@
       <c r="AE101" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A2:A81">
+  <sortState ref="A2:A65">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>